<commit_message>
reorganizing; gis consolidated to ../2_gis/
</commit_message>
<xml_diff>
--- a/data/landcover_id.xlsx
+++ b/data/landcover_id.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsz/Documents/UNIL/opfo_sampling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsz/Documents/unil/opfo_str_sampling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3342A905-73F4-6D4B-B3B6-C6CE36E5EBD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DB0F47-11FE-054D-82B5-D1C6E71A31EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="660" windowWidth="10000" windowHeight="16340" xr2:uid="{1513D67B-87A3-B041-8C2C-74300B6FD21A}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>LC</t>
   </si>
@@ -82,6 +76,45 @@
   </si>
   <si>
     <t>zalluviale</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>Canopy</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Mixed</t>
   </si>
 </sst>
 </file>
@@ -117,8 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,140 +467,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0A8A80-ADAB-104B-8568-17A5A6875564}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>